<commit_message>
Backup all CS3080 course files and utilities
- Added CLAUDE.md documentation for repository
- Added utility scripts for file management, MP3 organization, PDF/image processing
- Added Task_2 reports and deliverables
- Added pygame learning files and exercises
- Updated existing scripts and Excel files
- Added in-class exercises and homework files

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Task_2/authors.xlsx
+++ b/Task_2/authors.xlsx
@@ -425,17 +425,17 @@
       <c r="A1" t="inlineStr"/>
       <c r="B1" t="inlineStr">
         <is>
+          <t>Lei Zhang</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Dacheng Tao</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>Luc Van Gool</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Dacheng Tao</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Lei Zhang</t>
         </is>
       </c>
     </row>
@@ -446,13 +446,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C2" t="n">
         <v>13</v>
       </c>
       <c r="D2" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -462,13 +462,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C3" t="n">
         <v>22</v>
       </c>
       <c r="D3" t="n">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4">
@@ -478,13 +478,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C4" t="n">
         <v>14</v>
       </c>
       <c r="D4" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
@@ -494,13 +494,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C5" t="n">
         <v>49</v>
       </c>
       <c r="D5" t="n">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>